<commit_message>
Changed the path of excel
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestDataShareSkill.xlsx
+++ b/MarsFramework/ExcelData/TestDataShareSkill.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhya\source\repos\MarsFramework\MarsFramework\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPER\source\repos\piper9797\Skillwap_Test3(standard sprint)\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9272ECE-833C-43AE-9AC5-5DC008F12B22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1978C4-282C-43B3-836F-A275C34D5D7F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Url</t>
   </si>
@@ -51,18 +51,6 @@
     <t>ConfirmPswd</t>
   </si>
   <si>
-    <t>Venugan</t>
-  </si>
-  <si>
-    <t>Vidhya</t>
-  </si>
-  <si>
-    <t>vidhyav9@gmail.com</t>
-  </si>
-  <si>
-    <t>Ithika2015</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -78,64 +66,74 @@
     <t>Active</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Selenium</t>
-  </si>
-  <si>
-    <t>Would like to provide selenium training for beginners</t>
-  </si>
-  <si>
     <t>Skill-Exchange</t>
   </si>
   <si>
     <t>SubCategory</t>
   </si>
   <si>
-    <t>QA</t>
-  </si>
-  <si>
-    <t>Programming &amp; Tech</t>
+    <t>ServiceType</t>
+  </si>
+  <si>
+    <t>LocationType</t>
+  </si>
+  <si>
+    <t>Startdate</t>
+  </si>
+  <si>
+    <t>Enddate</t>
+  </si>
+  <si>
+    <t>Starttime</t>
+  </si>
+  <si>
+    <t>Endtime</t>
+  </si>
+  <si>
+    <t>SkillTrade</t>
+  </si>
+  <si>
+    <t>Selectday</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Thai boxing</t>
+  </si>
+  <si>
+    <t>Thai boxing exchanges Arts</t>
+  </si>
+  <si>
+    <t>Fun &amp; Lifestyle</t>
+  </si>
+  <si>
+    <t>Health, Nutrition &amp; Fitness</t>
   </si>
   <si>
     <t>One-off service</t>
-  </si>
-  <si>
-    <t>ServiceType</t>
-  </si>
-  <si>
-    <t>LocationType</t>
-  </si>
-  <si>
-    <t>Startdate</t>
-  </si>
-  <si>
-    <t>Enddate</t>
-  </si>
-  <si>
-    <t>Starttime</t>
-  </si>
-  <si>
-    <t>Endtime</t>
-  </si>
-  <si>
-    <t>SkillTrade</t>
-  </si>
-  <si>
-    <t>On-site</t>
-  </si>
-  <si>
-    <t>Performance Testing</t>
-  </si>
-  <si>
-    <t>Hidden</t>
-  </si>
-  <si>
-    <t>Selectday</t>
-  </si>
-  <si>
-    <t>Mon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fighting skill</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Online</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill-exchange</t>
+  </si>
+  <si>
+    <t>mvpstudio.qa@gmail.com</t>
+  </si>
+  <si>
+    <t>SydneyQa2018</t>
+  </si>
+  <si>
+    <t>Arts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -143,14 +141,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -159,6 +157,19 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Abadi Extra Light"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -192,13 +203,17 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -541,19 +556,19 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" customWidth="1"/>
+    <col min="2" max="2" width="22.73046875" customWidth="1"/>
+    <col min="3" max="3" width="27.86328125" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -570,27 +585,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
+    <row r="2" spans="1:5" ht="14.65" x14ac:dyDescent="0.45">
+      <c r="C2" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -603,14 +602,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="45.86328125" customWidth="1"/>
+    <col min="2" max="2" width="27.59765625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,25 +620,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.65" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" display="Test@123" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -647,125 +645,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="1" max="4" width="20.1328125" customWidth="1"/>
+    <col min="5" max="5" width="18.265625" customWidth="1"/>
+    <col min="6" max="6" width="24.86328125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="8" max="12" width="12.73046875" customWidth="1"/>
+    <col min="13" max="13" width="14.3984375" customWidth="1"/>
+    <col min="14" max="14" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.3984375" customWidth="1"/>
+    <col min="16" max="16" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:17" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="5">
+        <v>43567</v>
+      </c>
+      <c r="I2" s="6">
+        <v>43597</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="4">
-        <v>43567</v>
-      </c>
-      <c r="I2" s="3">
-        <v>43597</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="5">
+      <c r="K2" s="7">
         <v>0.75</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="7">
         <v>0.83333333333333337</v>
       </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="M2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>35</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>